<commit_message>
- fixed pporRFP associated .gb link, note: this is on FreeGenes side from their backend db.
</commit_message>
<xml_diff>
--- a/Open Reporters Collection/Open Reporters Collection.xlsx
+++ b/Open Reporters Collection/Open Reporters Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Open Reporters Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83F7EAC-2DF1-F04F-A0FA-0A99B6ADCF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D031137E-021D-4344-AFF5-50B1D548C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="2800" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7816" uniqueCount="7596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7816" uniqueCount="7597">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22892,6 +22892,9 @@
   </si>
   <si>
     <t>Takend from Open Reports Collection at FreeGenes</t>
+  </si>
+  <si>
+    <t>https://freegenes.github.io/genbank/BBF10K_003359.gb</t>
   </si>
 </sst>
 </file>
@@ -23231,7 +23234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23290,6 +23293,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23746,8 +23751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24113,7 +24118,7 @@
       <c r="F16" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="53" t="s">
         <v>7564</v>
       </c>
       <c r="H16" s="18"/>
@@ -24817,7 +24822,7 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="52" t="s">
         <v>7554</v>
       </c>
       <c r="B35" s="41" t="s">
@@ -24835,8 +24840,8 @@
       <c r="F35" s="18" t="s">
         <v>7529</v>
       </c>
-      <c r="G35" s="21" t="s">
-        <v>7581</v>
+      <c r="G35" s="53" t="s">
+        <v>7596</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="18" t="s">
@@ -26297,10 +26302,14 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G16" r:id="rId1" xr:uid="{7692EBD2-9493-AF46-88F0-C8F308979C1E}"/>
+    <hyperlink ref="G35" r:id="rId2" xr:uid="{5C757F9E-603B-E842-80F0-0AC3207601DE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>